<commit_message>
small change to make a test
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/Majors-pat.xlsx
+++ b/prerequisites/trial prereq/Majors-pat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jcuoncloud-my.sharepoint.com/personal/pangelini_johncabot_edu/Documents/Teaching/ResearchAssistantship/FA22-Elettra/advising/prerequisites/trial prereq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{0A31F5AE-A4FA-48FA-B252-2185755BC832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C41BF1-368A-4822-82BE-A7F100C14E60}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{0A31F5AE-A4FA-48FA-B252-2185755BC832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCCC7858-EA91-47AB-8C5C-CD65A76A04C0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{39B82AA1-F665-4363-970D-8821589D72FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
   <si>
     <t>Major Name</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Something</t>
+  </si>
+  <si>
+    <t>Other major</t>
+  </si>
+  <si>
+    <t>Something else</t>
   </si>
 </sst>
 </file>
@@ -799,10 +805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59450D2-57C3-49E6-BEAA-FC9212D01DEC}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1215,6 +1221,105 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>110</v>
+      </c>
+      <c r="E28">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>197</v>
+      </c>
+      <c r="E29">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>209</v>
+      </c>
+      <c r="E30">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>301</v>
+      </c>
+      <c r="E31">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>300</v>
+      </c>
+      <c r="E32">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>